<commit_message>
Fix: Correct binded variable
</commit_message>
<xml_diff>
--- a/web/tmp/report/transaction_report.xlsx
+++ b/web/tmp/report/transaction_report.xlsx
@@ -15,18 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>TRANSACTION REPORT</t>
   </si>
   <si>
-    <t xml:space="preserve">Transaction Date: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment Date: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Printed By: </t>
+    <t>Transaction Date</t>
+  </si>
+  <si>
+    <t>Payment Date</t>
+  </si>
+  <si>
+    <t>Printed By</t>
   </si>
   <si>
     <t>16/07/2024 - 17/07/2024</t>
@@ -39,12 +39,6 @@
   </si>
   <si>
     <t>Order No</t>
-  </si>
-  <si>
-    <t>Transaction Date</t>
-  </si>
-  <si>
-    <t>Payment Date</t>
   </si>
   <si>
     <t>Total Amount</t>
@@ -99,12 +93,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ffcdcdcd"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -137,7 +137,9 @@
   <cellXfs count="4">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -489,33 +491,33 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D7" s="3">
         <v>115000</v>
@@ -532,13 +534,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
         <v>145000</v>
@@ -555,7 +557,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>

</xml_diff>